<commit_message>
A&E lightning test cases
</commit_message>
<xml_diff>
--- a/resources/TestFiles/TestFileDraco.xlsx
+++ b/resources/TestFiles/TestFileDraco.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\manish9x\Git for Draco Nov 23\AccessandEntitlementsAutomation\resources\TestFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\manish9x\Git for Draco 2\AccessandEntitlementsAutomation\resources\TestFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18E6E0D3-A1B4-4038-9740-C4DBF650ADC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCB67734-9D6E-44AD-951C-64532F873B3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="530" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="586" uniqueCount="218">
   <si>
     <t>Users</t>
   </si>
@@ -601,15 +601,6 @@
     <t>Geo</t>
   </si>
   <si>
-    <t>End Customer Account</t>
-  </si>
-  <si>
-    <t>MSVP L1</t>
-  </si>
-  <si>
-    <t>Quote Owner</t>
-  </si>
-  <si>
     <t>TC0001_DRACO</t>
   </si>
   <si>
@@ -623,13 +614,103 @@
   </si>
   <si>
     <t>Intel*1234</t>
+  </si>
+  <si>
+    <t>First Name</t>
+  </si>
+  <si>
+    <t>Last Name</t>
+  </si>
+  <si>
+    <t>Account Name</t>
+  </si>
+  <si>
+    <t>Mr.</t>
+  </si>
+  <si>
+    <t>Automation</t>
+  </si>
+  <si>
+    <t>Samsung Corp</t>
+  </si>
+  <si>
+    <t>TC0002_DRACO</t>
+  </si>
+  <si>
+    <t>TC0004_DRACO</t>
+  </si>
+  <si>
+    <t>DummyTest201</t>
+  </si>
+  <si>
+    <t>auto201@mailinator.com</t>
+  </si>
+  <si>
+    <t>TC0003_DRACO</t>
+  </si>
+  <si>
+    <t>DummyTest202</t>
+  </si>
+  <si>
+    <t>auto202@mailinator.com</t>
+  </si>
+  <si>
+    <t>TC0005_DRACO</t>
+  </si>
+  <si>
+    <t>Exportcheck</t>
+  </si>
+  <si>
+    <t>contact01</t>
+  </si>
+  <si>
+    <t>exportcontactchecktc5@mailinator.com</t>
+  </si>
+  <si>
+    <t>Automation_DRACO_Test</t>
+  </si>
+  <si>
+    <t>TC0006_DRACO</t>
+  </si>
+  <si>
+    <t>contact02</t>
+  </si>
+  <si>
+    <t>exportcontact2checktc5@mailinator.com</t>
+  </si>
+  <si>
+    <t>TC0007_DRACO</t>
+  </si>
+  <si>
+    <t>season branch Ahemdabad</t>
+  </si>
+  <si>
+    <t>employee8pg8@mailinator.com</t>
+  </si>
+  <si>
+    <t>employee8</t>
+  </si>
+  <si>
+    <t>pg8</t>
+  </si>
+  <si>
+    <t>TC0008_DRACO</t>
+  </si>
+  <si>
+    <t>testautomationuser01contactdracodnt01@mailinator.com</t>
+  </si>
+  <si>
+    <t>Testautomationuser01</t>
+  </si>
+  <si>
+    <t>contactdracodnt01</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -663,12 +744,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10.5"/>
-      <color theme="1"/>
-      <name val="Segoe UI"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -732,7 +807,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -798,7 +873,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2960,7 +3034,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C2" sqref="C2"/>
+      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2989,29 +3063,29 @@
         <v>182</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="28" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" s="27" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="29"/>
-      <c r="D2" s="30"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="29"/>
       <c r="E2" s="1"/>
     </row>
-    <row r="3" spans="1:5" s="28" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" s="27" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="29" t="s">
-        <v>189</v>
-      </c>
-      <c r="D3" s="30" t="s">
-        <v>190</v>
+      <c r="C3" s="28" t="s">
+        <v>186</v>
+      </c>
+      <c r="D3" s="29" t="s">
+        <v>187</v>
       </c>
       <c r="E3" s="1"/>
     </row>
@@ -3028,24 +3102,25 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AE4A502-95AD-4FD1-BDAA-46A877825265}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="topRight" activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="14" style="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25" style="12" customWidth="1"/>
-    <col min="3" max="3" width="19.90625" style="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.7265625" style="12"/>
-    <col min="5" max="5" width="24.26953125" style="12" customWidth="1"/>
-    <col min="6" max="16384" width="8.7265625" style="12"/>
+    <col min="2" max="2" width="8.6328125" style="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.1796875" style="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="24.26953125" style="12" customWidth="1"/>
+    <col min="6" max="6" width="50.26953125" style="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.26953125" style="12" customWidth="1"/>
+    <col min="8" max="16384" width="8.7265625" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
         <v>53</v>
       </c>
@@ -3053,28 +3128,217 @@
         <v>52</v>
       </c>
       <c r="C1" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>188</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>189</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A2" s="5" t="s">
         <v>183</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="E1" s="10" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="17" x14ac:dyDescent="0.5">
-      <c r="A2" s="5" t="s">
-        <v>186</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="2"/>
+      <c r="C2" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A3" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A4" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A5" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A6" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A7" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A8" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A9" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>210</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F2" r:id="rId1" xr:uid="{A0F38C3F-8DD2-4A5B-B0BE-A9A204DE5552}"/>
+    <hyperlink ref="F3" r:id="rId2" xr:uid="{003F3375-0E0B-4FBE-897F-0D1C3190EF25}"/>
+    <hyperlink ref="F4" r:id="rId3" xr:uid="{A4A063C3-A3F2-4A81-AFD7-A9360C1CCA35}"/>
+    <hyperlink ref="F5" r:id="rId4" xr:uid="{1D011E03-1B83-48F4-BC9E-922C89469B8E}"/>
+    <hyperlink ref="F6" r:id="rId5" xr:uid="{D07E9337-898B-4595-AAFC-FEF9016D1536}"/>
+    <hyperlink ref="F7" r:id="rId6" xr:uid="{3C31350D-F3E5-4416-A82E-2C1F8B703053}"/>
+    <hyperlink ref="F8" r:id="rId7" xr:uid="{D07FB25C-8E9E-4D89-A9FE-08AF4E75E138}"/>
+    <hyperlink ref="F9" r:id="rId8" xr:uid="{F3CA88DC-5CF6-4A82-BDE4-6467C21716DF}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId9"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
EUM community + Functionality test cases
</commit_message>
<xml_diff>
--- a/resources/TestFiles/TestFileDraco.xlsx
+++ b/resources/TestFiles/TestFileDraco.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\manish9x\Git for Draco 2\AccessandEntitlementsAutomation\resources\TestFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCB67734-9D6E-44AD-951C-64532F873B3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D0150C4-3B53-4780-8A2F-F3A2B5070587}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="586" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="700" uniqueCount="273">
   <si>
     <t>Users</t>
   </si>
@@ -704,6 +704,171 @@
   </si>
   <si>
     <t>contactdracodnt01</t>
+  </si>
+  <si>
+    <t>TC0009_DRACO</t>
+  </si>
+  <si>
+    <t>automation</t>
+  </si>
+  <si>
+    <t>TC0010_DRACO</t>
+  </si>
+  <si>
+    <t>TC0011_DRACO</t>
+  </si>
+  <si>
+    <t>Non Existing Email</t>
+  </si>
+  <si>
+    <t>First Name 2</t>
+  </si>
+  <si>
+    <t>Last Name 2</t>
+  </si>
+  <si>
+    <t>Account Type</t>
+  </si>
+  <si>
+    <t>Agency</t>
+  </si>
+  <si>
+    <t>ext201</t>
+  </si>
+  <si>
+    <t>ext202</t>
+  </si>
+  <si>
+    <t>automationext201@mailinator.com</t>
+  </si>
+  <si>
+    <t>automationext202@mailinator.com</t>
+  </si>
+  <si>
+    <t>TC0012_DRACO</t>
+  </si>
+  <si>
+    <t>TC0013_DRACO</t>
+  </si>
+  <si>
+    <t>automation01exttc13@mailinator.com</t>
+  </si>
+  <si>
+    <t>automation01</t>
+  </si>
+  <si>
+    <t>exttc13</t>
+  </si>
+  <si>
+    <t>ext303</t>
+  </si>
+  <si>
+    <t>ext304</t>
+  </si>
+  <si>
+    <t>automationext303@mailinator.com</t>
+  </si>
+  <si>
+    <t>automationext304@mailinator.com</t>
+  </si>
+  <si>
+    <t>nonexisting10</t>
+  </si>
+  <si>
+    <t>nonexisting11</t>
+  </si>
+  <si>
+    <t>automationnonexisting10@mailinator.com</t>
+  </si>
+  <si>
+    <t>automationnonexisting11@mailinator.com</t>
+  </si>
+  <si>
+    <t>nonexistingexttc13</t>
+  </si>
+  <si>
+    <t>automation01nonexistingexttc13@mailinator.com</t>
+  </si>
+  <si>
+    <t>TC0015_DRACO</t>
+  </si>
+  <si>
+    <t>automation02</t>
+  </si>
+  <si>
+    <t>automation02exttc13@mailinator.com</t>
+  </si>
+  <si>
+    <t>automation02nonexistingexttc13@modi.com</t>
+  </si>
+  <si>
+    <t>Account Name 2</t>
+  </si>
+  <si>
+    <t>Samsung Agency</t>
+  </si>
+  <si>
+    <t>TC0016_DRACO</t>
+  </si>
+  <si>
+    <t>TC0017_DRACO</t>
+  </si>
+  <si>
+    <t>exttc17</t>
+  </si>
+  <si>
+    <t>automationexttc17@mailinator.com</t>
+  </si>
+  <si>
+    <t>nonexistingexttc17</t>
+  </si>
+  <si>
+    <t>Corporate</t>
+  </si>
+  <si>
+    <t>TC0018_DRACO</t>
+  </si>
+  <si>
+    <t>exttc18</t>
+  </si>
+  <si>
+    <t>automation41nonexistingexttc17@mailinator.com</t>
+  </si>
+  <si>
+    <t>automation41</t>
+  </si>
+  <si>
+    <t>automation18</t>
+  </si>
+  <si>
+    <t>automation18exttc18@mailinator.com</t>
+  </si>
+  <si>
+    <t>TC0014_DRACO</t>
+  </si>
+  <si>
+    <t>exttc14</t>
+  </si>
+  <si>
+    <t>automationexttc14@mailinator.com</t>
+  </si>
+  <si>
+    <t>automationnonexisting14@mailinator.com</t>
+  </si>
+  <si>
+    <t>nonexisting14</t>
+  </si>
+  <si>
+    <t>automationnonexistingexttc16@cream.com</t>
+  </si>
+  <si>
+    <t>nonexistingexttc16</t>
+  </si>
+  <si>
+    <t>Account Type 2</t>
+  </si>
+  <si>
+    <t>Account Name 3</t>
   </si>
 </sst>
 </file>
@@ -3034,7 +3199,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomRight" activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3102,11 +3267,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AE4A502-95AD-4FD1-BDAA-46A877825265}">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:N19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="G9" sqref="G9"/>
+      <pane xSplit="1" topLeftCell="I1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3117,10 +3282,14 @@
     <col min="4" max="5" width="24.26953125" style="12" customWidth="1"/>
     <col min="6" max="6" width="50.26953125" style="12" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="24.26953125" style="12" customWidth="1"/>
-    <col min="8" max="16384" width="8.7265625" style="12"/>
+    <col min="8" max="8" width="43.26953125" style="12" bestFit="1" customWidth="1"/>
+    <col min="9" max="11" width="24.26953125" style="12" customWidth="1"/>
+    <col min="12" max="12" width="27.36328125" style="12" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="24.26953125" style="12" customWidth="1"/>
+    <col min="15" max="16384" width="8.7265625" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
         <v>53</v>
       </c>
@@ -3142,8 +3311,29 @@
       <c r="G1" s="10" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H1" s="10" t="s">
+        <v>222</v>
+      </c>
+      <c r="I1" s="10" t="s">
+        <v>223</v>
+      </c>
+      <c r="J1" s="10" t="s">
+        <v>224</v>
+      </c>
+      <c r="K1" s="10" t="s">
+        <v>225</v>
+      </c>
+      <c r="L1" s="10" t="s">
+        <v>250</v>
+      </c>
+      <c r="M1" s="10" t="s">
+        <v>271</v>
+      </c>
+      <c r="N1" s="10" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
         <v>183</v>
       </c>
@@ -3165,8 +3355,15 @@
       <c r="G2" s="2" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H2" s="3"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
         <v>194</v>
       </c>
@@ -3188,8 +3385,15 @@
       <c r="G3" s="2" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H3" s="3"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
         <v>195</v>
       </c>
@@ -3211,8 +3415,15 @@
       <c r="G4" s="2" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H4" s="3"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
         <v>198</v>
       </c>
@@ -3234,8 +3445,15 @@
       <c r="G5" s="2" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H5" s="3"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
         <v>201</v>
       </c>
@@ -3257,8 +3475,15 @@
       <c r="G6" s="2" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H6" s="3"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
         <v>206</v>
       </c>
@@ -3280,8 +3505,15 @@
       <c r="G7" s="2" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H7" s="3"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
         <v>209</v>
       </c>
@@ -3303,8 +3535,15 @@
       <c r="G8" s="2" t="s">
         <v>210</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H8" s="3"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
         <v>214</v>
       </c>
@@ -3326,6 +3565,387 @@
       <c r="G9" s="2" t="s">
         <v>210</v>
       </c>
+      <c r="H9" s="3"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A10" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="H10" s="3"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
+      <c r="L10" s="2"/>
+      <c r="M10" s="2"/>
+      <c r="N10" s="2"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A11" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>230</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="H11" s="3"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
+      <c r="L11" s="2"/>
+      <c r="M11" s="2"/>
+      <c r="N11" s="2"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A12" s="5" t="s">
+        <v>221</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>238</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>242</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="K12" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="L12" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="M12" s="2"/>
+      <c r="N12" s="2"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A13" s="5" t="s">
+        <v>231</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="K13" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="L13" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="M13" s="2"/>
+      <c r="N13" s="2"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A14" s="5" t="s">
+        <v>232</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="K14" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="L14" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="M14" s="2"/>
+      <c r="N14" s="2"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A15" s="5" t="s">
+        <v>264</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="J15" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="K15" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="L15" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="M15" s="2"/>
+      <c r="N15" s="2"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A16" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>249</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="K16" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="L16" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="M16" s="2"/>
+      <c r="N16" s="2"/>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A17" s="5" t="s">
+        <v>252</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>269</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="J17" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="K17" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="L17" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="M17" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="N17" s="2" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A18" s="5" t="s">
+        <v>253</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>255</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>260</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="K18" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="L18" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="M18" s="2"/>
+      <c r="N18" s="2"/>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A19" s="5" t="s">
+        <v>258</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>263</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="H19" s="3"/>
+      <c r="I19" s="2"/>
+      <c r="J19" s="2"/>
+      <c r="K19" s="2"/>
+      <c r="L19" s="2"/>
+      <c r="M19" s="2"/>
+      <c r="N19" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -3337,8 +3957,25 @@
     <hyperlink ref="F7" r:id="rId6" xr:uid="{3C31350D-F3E5-4416-A82E-2C1F8B703053}"/>
     <hyperlink ref="F8" r:id="rId7" xr:uid="{D07FB25C-8E9E-4D89-A9FE-08AF4E75E138}"/>
     <hyperlink ref="F9" r:id="rId8" xr:uid="{F3CA88DC-5CF6-4A82-BDE4-6467C21716DF}"/>
+    <hyperlink ref="F10" r:id="rId9" xr:uid="{7D6E0C57-FA7B-402C-B65D-F96FBB9F3E2C}"/>
+    <hyperlink ref="F11" r:id="rId10" xr:uid="{09198764-D21C-409F-931A-B3A793E82926}"/>
+    <hyperlink ref="F12" r:id="rId11" xr:uid="{BD7E40A0-8F54-4067-BB87-69800194E50C}"/>
+    <hyperlink ref="H12" r:id="rId12" xr:uid="{AD9A1001-D204-4573-AA15-29F0747FEEBD}"/>
+    <hyperlink ref="F13" r:id="rId13" xr:uid="{AFBD5D07-D274-42A3-921E-09F8ADEBC371}"/>
+    <hyperlink ref="H13" r:id="rId14" xr:uid="{CBBBFA45-4D76-416F-BDE5-B9B4706F94C9}"/>
+    <hyperlink ref="F14" r:id="rId15" xr:uid="{650192EF-5F40-471A-897A-3541B9A389AD}"/>
+    <hyperlink ref="H14" r:id="rId16" xr:uid="{2CDFED2A-5CBF-4C39-87D0-6CAD53892994}"/>
+    <hyperlink ref="F16" r:id="rId17" xr:uid="{FB54A06C-30E3-4372-9304-54A30991E1EB}"/>
+    <hyperlink ref="H16" r:id="rId18" xr:uid="{C9EDE456-BDFE-4C93-88C9-33BDAE119A49}"/>
+    <hyperlink ref="F17" r:id="rId19" xr:uid="{3ED0E95F-3803-46A7-89EB-E09BBA8E309E}"/>
+    <hyperlink ref="F18" r:id="rId20" xr:uid="{1915ADDD-E0AA-4EDF-BFA2-3B67EEB7DAC8}"/>
+    <hyperlink ref="H18" r:id="rId21" xr:uid="{676479B4-BCB5-4F2E-BEE7-9CA8EC410B98}"/>
+    <hyperlink ref="F19" r:id="rId22" xr:uid="{DD7ECCF9-CE3C-4C34-9729-40F3A6F5D4BF}"/>
+    <hyperlink ref="F15" r:id="rId23" xr:uid="{332B3AFE-6B38-4382-A375-4C2003EF6166}"/>
+    <hyperlink ref="H15" r:id="rId24" xr:uid="{93857D19-0431-42BF-87C2-35743ECD0740}"/>
+    <hyperlink ref="H17" r:id="rId25" xr:uid="{77683C9B-7616-4541-9DA9-5C3DCED6A999}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId9"/>
+  <pageSetup orientation="portrait" r:id="rId26"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Committing Manage Personnel testcases' modules
</commit_message>
<xml_diff>
--- a/resources/TestFiles/TestFileDraco.xlsx
+++ b/resources/TestFiles/TestFileDraco.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\manish9x\Git for Draco 2\AccessandEntitlementsAutomation\resources\TestFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asuhassx\giteum\AccessandEntitlementsAutomation\resources\TestFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D0150C4-3B53-4780-8A2F-F3A2B5070587}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A60AD00-5573-47FB-883F-90431E19AA52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="700" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="652" uniqueCount="257">
   <si>
     <t>Users</t>
   </si>
@@ -610,272 +610,224 @@
     <t>User1 DEVINT</t>
   </si>
   <si>
+    <t>First Name</t>
+  </si>
+  <si>
+    <t>Last Name</t>
+  </si>
+  <si>
+    <t>Account Name</t>
+  </si>
+  <si>
+    <t>Mr.</t>
+  </si>
+  <si>
+    <t>Samsung Corp</t>
+  </si>
+  <si>
+    <t>TC0002_DRACO</t>
+  </si>
+  <si>
+    <t>TC0004_DRACO</t>
+  </si>
+  <si>
+    <t>TC0003_DRACO</t>
+  </si>
+  <si>
+    <t>TC0005_DRACO</t>
+  </si>
+  <si>
+    <t>Automation_DRACO_Test</t>
+  </si>
+  <si>
+    <t>TC0006_DRACO</t>
+  </si>
+  <si>
+    <t>TC0007_DRACO</t>
+  </si>
+  <si>
+    <t>TC0008_DRACO</t>
+  </si>
+  <si>
+    <t>TC0009_DRACO</t>
+  </si>
+  <si>
+    <t>TC0010_DRACO</t>
+  </si>
+  <si>
+    <t>TC0011_DRACO</t>
+  </si>
+  <si>
+    <t>Non Existing Email</t>
+  </si>
+  <si>
+    <t>First Name 2</t>
+  </si>
+  <si>
+    <t>Last Name 2</t>
+  </si>
+  <si>
+    <t>Account Type</t>
+  </si>
+  <si>
+    <t>TC0012_DRACO</t>
+  </si>
+  <si>
+    <t>TC0013_DRACO</t>
+  </si>
+  <si>
+    <t>TC0015_DRACO</t>
+  </si>
+  <si>
+    <t>Account Name 2</t>
+  </si>
+  <si>
+    <t>TC0016_DRACO</t>
+  </si>
+  <si>
+    <t>TC0017_DRACO</t>
+  </si>
+  <si>
+    <t>Corporate</t>
+  </si>
+  <si>
+    <t>TC0018_DRACO</t>
+  </si>
+  <si>
+    <t>TC0014_DRACO</t>
+  </si>
+  <si>
+    <t>Account Type 2</t>
+  </si>
+  <si>
+    <t>Account Name 3</t>
+  </si>
+  <si>
+    <t>TC0019_DRACO</t>
+  </si>
+  <si>
+    <t>Existing Email</t>
+  </si>
+  <si>
+    <t>TC0020_DRACO</t>
+  </si>
+  <si>
     <t>12004853@intel.com.crm.crmqa3</t>
   </si>
   <si>
     <t>Intel*1234</t>
   </si>
   <si>
-    <t>First Name</t>
-  </si>
-  <si>
-    <t>Last Name</t>
-  </si>
-  <si>
-    <t>Account Name</t>
-  </si>
-  <si>
-    <t>Mr.</t>
-  </si>
-  <si>
-    <t>Automation</t>
-  </si>
-  <si>
-    <t>Samsung Corp</t>
-  </si>
-  <si>
-    <t>TC0002_DRACO</t>
-  </si>
-  <si>
-    <t>TC0004_DRACO</t>
-  </si>
-  <si>
-    <t>DummyTest201</t>
-  </si>
-  <si>
-    <t>auto201@mailinator.com</t>
-  </si>
-  <si>
-    <t>TC0003_DRACO</t>
-  </si>
-  <si>
-    <t>DummyTest202</t>
-  </si>
-  <si>
-    <t>auto202@mailinator.com</t>
-  </si>
-  <si>
-    <t>TC0005_DRACO</t>
-  </si>
-  <si>
-    <t>Exportcheck</t>
-  </si>
-  <si>
-    <t>contact01</t>
-  </si>
-  <si>
-    <t>exportcontactchecktc5@mailinator.com</t>
-  </si>
-  <si>
-    <t>Automation_DRACO_Test</t>
-  </si>
-  <si>
-    <t>TC0006_DRACO</t>
-  </si>
-  <si>
-    <t>contact02</t>
-  </si>
-  <si>
-    <t>exportcontact2checktc5@mailinator.com</t>
-  </si>
-  <si>
-    <t>TC0007_DRACO</t>
-  </si>
-  <si>
-    <t>season branch Ahemdabad</t>
-  </si>
-  <si>
-    <t>employee8pg8@mailinator.com</t>
-  </si>
-  <si>
-    <t>employee8</t>
-  </si>
-  <si>
-    <t>pg8</t>
-  </si>
-  <si>
-    <t>TC0008_DRACO</t>
-  </si>
-  <si>
-    <t>testautomationuser01contactdracodnt01@mailinator.com</t>
-  </si>
-  <si>
-    <t>Testautomationuser01</t>
-  </si>
-  <si>
-    <t>contactdracodnt01</t>
-  </si>
-  <si>
-    <t>TC0009_DRACO</t>
-  </si>
-  <si>
-    <t>automation</t>
-  </si>
-  <si>
-    <t>TC0010_DRACO</t>
-  </si>
-  <si>
-    <t>TC0011_DRACO</t>
-  </si>
-  <si>
-    <t>Non Existing Email</t>
-  </si>
-  <si>
-    <t>First Name 2</t>
-  </si>
-  <si>
-    <t>Last Name 2</t>
-  </si>
-  <si>
-    <t>Account Type</t>
-  </si>
-  <si>
-    <t>Agency</t>
-  </si>
-  <si>
-    <t>ext201</t>
-  </si>
-  <si>
-    <t>ext202</t>
-  </si>
-  <si>
-    <t>automationext201@mailinator.com</t>
-  </si>
-  <si>
-    <t>automationext202@mailinator.com</t>
-  </si>
-  <si>
-    <t>TC0012_DRACO</t>
-  </si>
-  <si>
-    <t>TC0013_DRACO</t>
-  </si>
-  <si>
-    <t>automation01exttc13@mailinator.com</t>
-  </si>
-  <si>
-    <t>automation01</t>
-  </si>
-  <si>
-    <t>exttc13</t>
-  </si>
-  <si>
-    <t>ext303</t>
-  </si>
-  <si>
-    <t>ext304</t>
-  </si>
-  <si>
-    <t>automationext303@mailinator.com</t>
-  </si>
-  <si>
-    <t>automationext304@mailinator.com</t>
-  </si>
-  <si>
-    <t>nonexisting10</t>
-  </si>
-  <si>
-    <t>nonexisting11</t>
-  </si>
-  <si>
-    <t>automationnonexisting10@mailinator.com</t>
-  </si>
-  <si>
-    <t>automationnonexisting11@mailinator.com</t>
-  </si>
-  <si>
-    <t>nonexistingexttc13</t>
-  </si>
-  <si>
-    <t>automation01nonexistingexttc13@mailinator.com</t>
-  </si>
-  <si>
-    <t>TC0015_DRACO</t>
-  </si>
-  <si>
-    <t>automation02</t>
-  </si>
-  <si>
-    <t>automation02exttc13@mailinator.com</t>
-  </si>
-  <si>
-    <t>automation02nonexistingexttc13@modi.com</t>
-  </si>
-  <si>
-    <t>Account Name 2</t>
-  </si>
-  <si>
-    <t>Samsung Agency</t>
-  </si>
-  <si>
-    <t>TC0016_DRACO</t>
-  </si>
-  <si>
-    <t>TC0017_DRACO</t>
-  </si>
-  <si>
-    <t>exttc17</t>
-  </si>
-  <si>
-    <t>automationexttc17@mailinator.com</t>
-  </si>
-  <si>
-    <t>nonexistingexttc17</t>
-  </si>
-  <si>
-    <t>Corporate</t>
-  </si>
-  <si>
-    <t>TC0018_DRACO</t>
-  </si>
-  <si>
-    <t>exttc18</t>
-  </si>
-  <si>
-    <t>automation41nonexistingexttc17@mailinator.com</t>
-  </si>
-  <si>
-    <t>automation41</t>
-  </si>
-  <si>
-    <t>automation18</t>
-  </si>
-  <si>
-    <t>automation18exttc18@mailinator.com</t>
-  </si>
-  <si>
-    <t>TC0014_DRACO</t>
-  </si>
-  <si>
-    <t>exttc14</t>
-  </si>
-  <si>
-    <t>automationexttc14@mailinator.com</t>
-  </si>
-  <si>
-    <t>automationnonexisting14@mailinator.com</t>
-  </si>
-  <si>
-    <t>nonexisting14</t>
-  </si>
-  <si>
-    <t>automationnonexistingexttc16@cream.com</t>
-  </si>
-  <si>
-    <t>nonexistingexttc16</t>
-  </si>
-  <si>
-    <t>Account Type 2</t>
-  </si>
-  <si>
-    <t>Account Name 3</t>
+    <t>Automationccprun01</t>
+  </si>
+  <si>
+    <t>User01</t>
+  </si>
+  <si>
+    <t>Automationexistingcontact</t>
+  </si>
+  <si>
+    <t>testingaande</t>
+  </si>
+  <si>
+    <t>automationexistingcontact001@mailinator.com</t>
+  </si>
+  <si>
+    <t>AutomationPSGcontact001</t>
+  </si>
+  <si>
+    <t>testexistingande</t>
+  </si>
+  <si>
+    <t>automationpsgcontact001@mailinator.com</t>
+  </si>
+  <si>
+    <t>AutomationPSGrun01</t>
+  </si>
+  <si>
+    <t>Automationeumccp01</t>
+  </si>
+  <si>
+    <t>Usereum01</t>
+  </si>
+  <si>
+    <t>nonexistingemailfirsteum87@mailinator.com</t>
+  </si>
+  <si>
+    <t>EumGAcontact01</t>
+  </si>
+  <si>
+    <t>CCPextuser01</t>
+  </si>
+  <si>
+    <t>Automationeumccp02</t>
+  </si>
+  <si>
+    <t>Usereum02</t>
+  </si>
+  <si>
+    <t>test_qa0922@mailinator.com</t>
+  </si>
+  <si>
+    <t>Automationeumccp04</t>
+  </si>
+  <si>
+    <t>Usereum03</t>
+  </si>
+  <si>
+    <t>Usereum04</t>
+  </si>
+  <si>
+    <t>nonexistingemailfirsteum885@mailinator.com</t>
+  </si>
+  <si>
+    <t>EumGAcontact02</t>
+  </si>
+  <si>
+    <t>CCPextuser02</t>
+  </si>
+  <si>
+    <t>TC0021_DRACO</t>
+  </si>
+  <si>
+    <t>TC0022_DRACO</t>
+  </si>
+  <si>
+    <t>TC0023_DRACO</t>
+  </si>
+  <si>
+    <t>TC0024_DRACO</t>
+  </si>
+  <si>
+    <t>TC0025_DRACO</t>
+  </si>
+  <si>
+    <t>AutomationMPdraco</t>
+  </si>
+  <si>
+    <t>Useripa01</t>
+  </si>
+  <si>
+    <t>Season Branch Pune</t>
+  </si>
+  <si>
+    <t>Filter</t>
+  </si>
+  <si>
+    <t>testcontactinvite43@ipa.com</t>
+  </si>
+  <si>
+    <t>AutomationMPdraco2</t>
+  </si>
+  <si>
+    <t>Useripa02</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -910,6 +862,19 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="6"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color rgb="FF262626"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -931,7 +896,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -967,12 +932,23 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -1042,6 +1018,16 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3247,31 +3233,28 @@
         <v>18</v>
       </c>
       <c r="C3" s="28" t="s">
-        <v>186</v>
+        <v>220</v>
       </c>
       <c r="D3" s="29" t="s">
-        <v>187</v>
+        <v>221</v>
       </c>
       <c r="E3" s="1"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:E3" xr:uid="{B30C7179-49C6-4CE4-9EE3-050BEF570246}"/>
   <phoneticPr fontId="3" type="noConversion"/>
-  <hyperlinks>
-    <hyperlink ref="C3" r:id="rId1" xr:uid="{17AAB3BA-1511-4C03-A49A-C595A54450F1}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AE4A502-95AD-4FD1-BDAA-46A877825265}">
-  <dimension ref="A1:N19"/>
+  <dimension ref="A1:P26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="I1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="K17" sqref="K17"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3286,10 +3269,12 @@
     <col min="9" max="11" width="24.26953125" style="12" customWidth="1"/>
     <col min="12" max="12" width="27.36328125" style="12" bestFit="1" customWidth="1"/>
     <col min="13" max="14" width="24.26953125" style="12" customWidth="1"/>
-    <col min="15" max="16384" width="8.7265625" style="12"/>
+    <col min="15" max="15" width="36.54296875" style="12" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.26953125" style="12" customWidth="1"/>
+    <col min="17" max="16384" width="8.7265625" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
         <v>53</v>
       </c>
@@ -3300,40 +3285,46 @@
         <v>22</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="F1" s="10" t="s">
         <v>6</v>
       </c>
       <c r="G1" s="10" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="H1" s="10" t="s">
-        <v>222</v>
+        <v>202</v>
       </c>
       <c r="I1" s="10" t="s">
-        <v>223</v>
+        <v>203</v>
       </c>
       <c r="J1" s="10" t="s">
-        <v>224</v>
+        <v>204</v>
       </c>
       <c r="K1" s="10" t="s">
-        <v>225</v>
+        <v>205</v>
       </c>
       <c r="L1" s="10" t="s">
-        <v>250</v>
+        <v>209</v>
       </c>
       <c r="M1" s="10" t="s">
-        <v>271</v>
+        <v>215</v>
       </c>
       <c r="N1" s="10" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+        <v>216</v>
+      </c>
+      <c r="O1" s="10" t="s">
+        <v>218</v>
+      </c>
+      <c r="P1" s="34" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
         <v>183</v>
       </c>
@@ -3341,641 +3332,429 @@
         <v>184</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>222</v>
+      </c>
+      <c r="E2" s="30" t="s">
+        <v>223</v>
+      </c>
+      <c r="F2" s="12" t="str">
+        <f>_xlfn.CONCAT(D2,E2,"@mailinator.com")</f>
+        <v>Automationccprun01User01@mailinator.com</v>
+      </c>
+      <c r="G2" s="31" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A3" s="5" t="s">
         <v>191</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>197</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="H2" s="3"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
-      <c r="M2" s="2"/>
-      <c r="N2" s="2"/>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A3" s="5" t="s">
-        <v>194</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>184</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="D3" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="D3" s="31" t="s">
+        <v>224</v>
+      </c>
+      <c r="E3" s="31" t="s">
+        <v>225</v>
+      </c>
+      <c r="F3" s="32" t="s">
+        <v>226</v>
+      </c>
+      <c r="G3" s="31" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A4" s="5" t="s">
         <v>192</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>197</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="H3" s="3"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-      <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
-      <c r="N3" s="2"/>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A4" s="5" t="s">
-        <v>195</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>184</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>200</v>
-      </c>
-      <c r="G4" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>230</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>223</v>
+      </c>
+      <c r="F4" s="12" t="str">
+        <f>_xlfn.CONCAT(D4,E4,"@mailinator.com")</f>
+        <v>AutomationPSGrun01User01@mailinator.com</v>
+      </c>
+      <c r="G4" s="31" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A5" s="5" t="s">
         <v>193</v>
-      </c>
-      <c r="H4" s="3"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
-      <c r="L4" s="2"/>
-      <c r="M4" s="2"/>
-      <c r="N4" s="2"/>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A5" s="5" t="s">
-        <v>198</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>184</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>200</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="H5" s="3"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
-      <c r="L5" s="2"/>
-      <c r="M5" s="2"/>
-      <c r="N5" s="2"/>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
+        <v>189</v>
+      </c>
+      <c r="D5" s="31" t="s">
+        <v>227</v>
+      </c>
+      <c r="E5" s="31" t="s">
+        <v>228</v>
+      </c>
+      <c r="F5" s="32" t="s">
+        <v>229</v>
+      </c>
+      <c r="G5" s="31" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>184</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>207</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>208</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>205</v>
-      </c>
-      <c r="H6" s="3"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
-      <c r="L6" s="2"/>
-      <c r="M6" s="2"/>
-      <c r="N6" s="2"/>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
-        <v>206</v>
+        <v>196</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>184</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>204</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>205</v>
-      </c>
-      <c r="H7" s="3"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
-      <c r="K7" s="2"/>
-      <c r="L7" s="2"/>
-      <c r="M7" s="2"/>
-      <c r="N7" s="2"/>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
-        <v>209</v>
+        <v>197</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>184</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>212</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>213</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>211</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>210</v>
-      </c>
-      <c r="H8" s="3"/>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
-      <c r="K8" s="2"/>
-      <c r="L8" s="2"/>
-      <c r="M8" s="2"/>
-      <c r="N8" s="2"/>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
-        <v>214</v>
+        <v>198</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>184</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>217</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>215</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>210</v>
-      </c>
-      <c r="H9" s="3"/>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
-      <c r="K9" s="2"/>
-      <c r="L9" s="2"/>
-      <c r="M9" s="2"/>
-      <c r="N9" s="2"/>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
-        <v>218</v>
+        <v>199</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>184</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>219</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>227</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>229</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>210</v>
-      </c>
-      <c r="H10" s="3"/>
-      <c r="I10" s="2"/>
-      <c r="J10" s="2"/>
-      <c r="K10" s="2"/>
-      <c r="L10" s="2"/>
-      <c r="M10" s="2"/>
-      <c r="N10" s="2"/>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
+        <v>189</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>231</v>
+      </c>
+      <c r="E10" s="12" t="s">
+        <v>232</v>
+      </c>
+      <c r="F10" s="12" t="str">
+        <f>_xlfn.CONCAT(D10,E10,"@mailinator.com")</f>
+        <v>Automationeumccp01Usereum01@mailinator.com</v>
+      </c>
+      <c r="G10" s="12" t="s">
+        <v>190</v>
+      </c>
+      <c r="H10" s="32" t="s">
+        <v>233</v>
+      </c>
+      <c r="I10" s="12" t="s">
+        <v>234</v>
+      </c>
+      <c r="J10" s="12" t="s">
+        <v>235</v>
+      </c>
+      <c r="K10" s="12" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
-        <v>220</v>
+        <v>200</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>184</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>219</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>228</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>230</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>210</v>
-      </c>
-      <c r="H11" s="3"/>
-      <c r="I11" s="2"/>
-      <c r="J11" s="2"/>
-      <c r="K11" s="2"/>
-      <c r="L11" s="2"/>
-      <c r="M11" s="2"/>
-      <c r="N11" s="2"/>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
+        <v>189</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>236</v>
+      </c>
+      <c r="E11" s="12" t="s">
+        <v>237</v>
+      </c>
+      <c r="F11" s="12" t="str">
+        <f>_xlfn.CONCAT(D11,E11,"@mailinator.com")</f>
+        <v>Automationeumccp02Usereum02@mailinator.com</v>
+      </c>
+      <c r="G11" s="12" t="s">
+        <v>190</v>
+      </c>
+      <c r="H11" s="32" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="s">
-        <v>221</v>
+        <v>201</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>184</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>219</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>236</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>238</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="H12" s="3" t="s">
-        <v>242</v>
-      </c>
-      <c r="I12" s="2" t="s">
-        <v>219</v>
-      </c>
-      <c r="J12" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="E12" s="12" t="s">
         <v>240</v>
       </c>
-      <c r="K12" s="2" t="s">
-        <v>226</v>
-      </c>
-      <c r="L12" s="2" t="s">
-        <v>251</v>
-      </c>
-      <c r="M12" s="2"/>
-      <c r="N12" s="2"/>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="F12" s="12" t="str">
+        <f t="shared" ref="F12:F13" si="0">_xlfn.CONCAT(D12,E12,"@mailinator.com")</f>
+        <v>Usereum03@mailinator.com</v>
+      </c>
+      <c r="G12" s="12" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
-        <v>231</v>
+        <v>206</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>184</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>219</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>237</v>
-      </c>
-      <c r="F13" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="D13" s="12" t="s">
         <v>239</v>
       </c>
-      <c r="G13" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="H13" s="3" t="s">
+      <c r="E13" s="12" t="s">
+        <v>241</v>
+      </c>
+      <c r="F13" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v>Automationeumccp04Usereum04@mailinator.com</v>
+      </c>
+      <c r="G13" s="12" t="s">
+        <v>190</v>
+      </c>
+      <c r="H13" s="32" t="s">
+        <v>242</v>
+      </c>
+      <c r="I13" s="12" t="s">
         <v>243</v>
       </c>
-      <c r="I13" s="2" t="s">
-        <v>219</v>
-      </c>
-      <c r="J13" s="2" t="s">
-        <v>241</v>
-      </c>
-      <c r="K13" s="2" t="s">
-        <v>257</v>
-      </c>
-      <c r="L13" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="M13" s="2"/>
-      <c r="N13" s="2"/>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="J13" s="12" t="s">
+        <v>244</v>
+      </c>
+      <c r="K13" s="12" t="s">
+        <v>212</v>
+      </c>
+      <c r="L13" s="12" t="s">
+        <v>190</v>
+      </c>
+      <c r="M13" s="12" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A14" s="5" t="s">
-        <v>232</v>
+        <v>207</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>184</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>234</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>235</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>233</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="H14" s="3" t="s">
-        <v>245</v>
-      </c>
-      <c r="I14" s="2" t="s">
-        <v>234</v>
-      </c>
-      <c r="J14" s="2" t="s">
-        <v>244</v>
-      </c>
-      <c r="K14" s="2" t="s">
-        <v>257</v>
-      </c>
-      <c r="L14" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="M14" s="2"/>
-      <c r="N14" s="2"/>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A15" s="5" t="s">
-        <v>264</v>
+        <v>214</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>184</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>219</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>265</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>266</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="H15" s="3" t="s">
-        <v>267</v>
-      </c>
-      <c r="I15" s="2" t="s">
-        <v>219</v>
-      </c>
-      <c r="J15" s="2" t="s">
-        <v>268</v>
-      </c>
-      <c r="K15" s="2" t="s">
-        <v>226</v>
-      </c>
-      <c r="L15" s="2" t="s">
-        <v>251</v>
-      </c>
-      <c r="M15" s="2"/>
-      <c r="N15" s="2"/>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A16" s="5" t="s">
-        <v>246</v>
+        <v>208</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>184</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>247</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>235</v>
-      </c>
-      <c r="F16" s="3" t="s">
-        <v>248</v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="H16" s="3" t="s">
-        <v>249</v>
-      </c>
-      <c r="I16" s="2" t="s">
-        <v>247</v>
-      </c>
-      <c r="J16" s="2" t="s">
-        <v>244</v>
-      </c>
-      <c r="K16" s="2" t="s">
-        <v>226</v>
-      </c>
-      <c r="L16" s="2" t="s">
-        <v>251</v>
-      </c>
-      <c r="M16" s="2"/>
-      <c r="N16" s="2"/>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A17" s="5" t="s">
-        <v>252</v>
+        <v>210</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>184</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>247</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>235</v>
-      </c>
-      <c r="F17" s="3" t="s">
-        <v>248</v>
-      </c>
-      <c r="G17" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="H17" s="3" t="s">
-        <v>269</v>
-      </c>
-      <c r="I17" s="2" t="s">
-        <v>219</v>
-      </c>
-      <c r="J17" s="2" t="s">
-        <v>270</v>
-      </c>
-      <c r="K17" s="2" t="s">
-        <v>257</v>
-      </c>
-      <c r="L17" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="M17" s="2" t="s">
-        <v>226</v>
-      </c>
-      <c r="N17" s="2" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A18" s="5" t="s">
-        <v>253</v>
+        <v>211</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>184</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>219</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>254</v>
-      </c>
-      <c r="F18" s="3" t="s">
-        <v>255</v>
-      </c>
-      <c r="G18" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="H18" s="3" t="s">
-        <v>260</v>
-      </c>
-      <c r="I18" s="2" t="s">
-        <v>261</v>
-      </c>
-      <c r="J18" s="2" t="s">
-        <v>256</v>
-      </c>
-      <c r="K18" s="2" t="s">
-        <v>257</v>
-      </c>
-      <c r="L18" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="M18" s="2"/>
-      <c r="N18" s="2"/>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A19" s="5" t="s">
-        <v>258</v>
+        <v>213</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>184</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>262</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>259</v>
-      </c>
-      <c r="F19" s="3" t="s">
-        <v>263</v>
-      </c>
-      <c r="G19" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="H19" s="3"/>
-      <c r="I19" s="2"/>
-      <c r="J19" s="2"/>
-      <c r="K19" s="2"/>
-      <c r="L19" s="2"/>
-      <c r="M19" s="2"/>
-      <c r="N19" s="2"/>
+        <v>189</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A20" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A21" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A22" s="33" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A23" s="33" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A24" s="33" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" ht="20" x14ac:dyDescent="0.35">
+      <c r="A25" s="33" t="s">
+        <v>248</v>
+      </c>
+      <c r="B25" s="12" t="s">
+        <v>184</v>
+      </c>
+      <c r="C25" s="12" t="s">
+        <v>189</v>
+      </c>
+      <c r="D25" s="12" t="s">
+        <v>255</v>
+      </c>
+      <c r="E25" s="30" t="s">
+        <v>256</v>
+      </c>
+      <c r="F25" s="12" t="str">
+        <f>_xlfn.CONCAT(D25,E25,"@mailinator.com")</f>
+        <v>AutomationMPdraco2Useripa02@mailinator.com</v>
+      </c>
+      <c r="G25" s="30" t="s">
+        <v>252</v>
+      </c>
+      <c r="P25" s="35" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" ht="30" x14ac:dyDescent="0.35">
+      <c r="A26" s="33" t="s">
+        <v>249</v>
+      </c>
+      <c r="B26" s="12" t="s">
+        <v>184</v>
+      </c>
+      <c r="C26" s="12" t="s">
+        <v>189</v>
+      </c>
+      <c r="D26" s="12" t="s">
+        <v>250</v>
+      </c>
+      <c r="E26" s="30" t="s">
+        <v>251</v>
+      </c>
+      <c r="F26" s="12" t="str">
+        <f>_xlfn.CONCAT(D26,E26,"@mailinator.com")</f>
+        <v>AutomationMPdracoUseripa01@mailinator.com</v>
+      </c>
+      <c r="G26" s="30" t="s">
+        <v>252</v>
+      </c>
+      <c r="P26" s="35" t="s">
+        <v>254</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" xr:uid="{A0F38C3F-8DD2-4A5B-B0BE-A9A204DE5552}"/>
-    <hyperlink ref="F3" r:id="rId2" xr:uid="{003F3375-0E0B-4FBE-897F-0D1C3190EF25}"/>
-    <hyperlink ref="F4" r:id="rId3" xr:uid="{A4A063C3-A3F2-4A81-AFD7-A9360C1CCA35}"/>
-    <hyperlink ref="F5" r:id="rId4" xr:uid="{1D011E03-1B83-48F4-BC9E-922C89469B8E}"/>
-    <hyperlink ref="F6" r:id="rId5" xr:uid="{D07E9337-898B-4595-AAFC-FEF9016D1536}"/>
-    <hyperlink ref="F7" r:id="rId6" xr:uid="{3C31350D-F3E5-4416-A82E-2C1F8B703053}"/>
-    <hyperlink ref="F8" r:id="rId7" xr:uid="{D07FB25C-8E9E-4D89-A9FE-08AF4E75E138}"/>
-    <hyperlink ref="F9" r:id="rId8" xr:uid="{F3CA88DC-5CF6-4A82-BDE4-6467C21716DF}"/>
-    <hyperlink ref="F10" r:id="rId9" xr:uid="{7D6E0C57-FA7B-402C-B65D-F96FBB9F3E2C}"/>
-    <hyperlink ref="F11" r:id="rId10" xr:uid="{09198764-D21C-409F-931A-B3A793E82926}"/>
-    <hyperlink ref="F12" r:id="rId11" xr:uid="{BD7E40A0-8F54-4067-BB87-69800194E50C}"/>
-    <hyperlink ref="H12" r:id="rId12" xr:uid="{AD9A1001-D204-4573-AA15-29F0747FEEBD}"/>
-    <hyperlink ref="F13" r:id="rId13" xr:uid="{AFBD5D07-D274-42A3-921E-09F8ADEBC371}"/>
-    <hyperlink ref="H13" r:id="rId14" xr:uid="{CBBBFA45-4D76-416F-BDE5-B9B4706F94C9}"/>
-    <hyperlink ref="F14" r:id="rId15" xr:uid="{650192EF-5F40-471A-897A-3541B9A389AD}"/>
-    <hyperlink ref="H14" r:id="rId16" xr:uid="{2CDFED2A-5CBF-4C39-87D0-6CAD53892994}"/>
-    <hyperlink ref="F16" r:id="rId17" xr:uid="{FB54A06C-30E3-4372-9304-54A30991E1EB}"/>
-    <hyperlink ref="H16" r:id="rId18" xr:uid="{C9EDE456-BDFE-4C93-88C9-33BDAE119A49}"/>
-    <hyperlink ref="F17" r:id="rId19" xr:uid="{3ED0E95F-3803-46A7-89EB-E09BBA8E309E}"/>
-    <hyperlink ref="F18" r:id="rId20" xr:uid="{1915ADDD-E0AA-4EDF-BFA2-3B67EEB7DAC8}"/>
-    <hyperlink ref="H18" r:id="rId21" xr:uid="{676479B4-BCB5-4F2E-BEE7-9CA8EC410B98}"/>
-    <hyperlink ref="F19" r:id="rId22" xr:uid="{DD7ECCF9-CE3C-4C34-9729-40F3A6F5D4BF}"/>
-    <hyperlink ref="F15" r:id="rId23" xr:uid="{332B3AFE-6B38-4382-A375-4C2003EF6166}"/>
-    <hyperlink ref="H15" r:id="rId24" xr:uid="{93857D19-0431-42BF-87C2-35743ECD0740}"/>
-    <hyperlink ref="H17" r:id="rId25" xr:uid="{77683C9B-7616-4541-9DA9-5C3DCED6A999}"/>
+    <hyperlink ref="F3" r:id="rId1" display="mailto:automationexistingcontact001@mailinator.com" xr:uid="{4A32C8CA-7755-49D2-A82C-F1CB1B382639}"/>
+    <hyperlink ref="F5" r:id="rId2" display="mailto:automationpsgcontact001@mailinator.com" xr:uid="{FC9FBAD0-E30D-4E7A-A705-7968A0E1C910}"/>
+    <hyperlink ref="H10" r:id="rId3" xr:uid="{DD0408AB-2BA5-4990-B211-0DF01180EEC9}"/>
+    <hyperlink ref="H11" r:id="rId4" display="mailto:test_qa0922@mailinator.com" xr:uid="{F8176DC2-7FD5-4C57-A0BD-03F4F7642923}"/>
+    <hyperlink ref="H13" r:id="rId5" xr:uid="{47E4F6EA-292A-4519-B99F-6843185CD22E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId26"/>
+  <pageSetup orientation="portrait" r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Commit Changes in DRACO
</commit_message>
<xml_diff>
--- a/resources/TestFiles/TestFileDraco.xlsx
+++ b/resources/TestFiles/TestFileDraco.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asuhassx\giteum\AccessandEntitlementsAutomation\resources\TestFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amartyax\gitDRACOApr10\AccessandEntitlementsAutomation\resources\TestFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A60AD00-5573-47FB-883F-90431E19AA52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ABF9BB0-535F-4801-8291-7B7EFE29DD4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="InternalUserData" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="652" uniqueCount="257">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="768" uniqueCount="298">
   <si>
     <t>Users</t>
   </si>
@@ -712,12 +712,6 @@
     <t>TC0020_DRACO</t>
   </si>
   <si>
-    <t>12004853@intel.com.crm.crmqa3</t>
-  </si>
-  <si>
-    <t>Intel*1234</t>
-  </si>
-  <si>
     <t>Automationccprun01</t>
   </si>
   <si>
@@ -821,6 +815,136 @@
   </si>
   <si>
     <t>Useripa02</t>
+  </si>
+  <si>
+    <t>TC0041_DRACO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">testself </t>
+  </si>
+  <si>
+    <t>nuna19123</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+testselfnuna19123@mail7.io</t>
+  </si>
+  <si>
+    <t>testaccount19123</t>
+  </si>
+  <si>
+    <t>automatedtestcasesusermpnewinvite6@mailinator.com</t>
+  </si>
+  <si>
+    <t>India</t>
+  </si>
+  <si>
+    <t>TC0042_DRACO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Season_PA </t>
+  </si>
+  <si>
+    <t>first</t>
+  </si>
+  <si>
+    <t>sopune1@lpql.com</t>
+  </si>
+  <si>
+    <t>testepum</t>
+  </si>
+  <si>
+    <t>one</t>
+  </si>
+  <si>
+    <t>testepumobm1@mail.com</t>
+  </si>
+  <si>
+    <t>TC0043_DRACO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test </t>
+  </si>
+  <si>
+    <t>ccpafffs</t>
+  </si>
+  <si>
+    <t>testccp011801@mailinator.com</t>
+  </si>
+  <si>
+    <t>TC0044_DRACO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">testent40 </t>
+  </si>
+  <si>
+    <t>check40</t>
+  </si>
+  <si>
+    <t>update_testent40check40@mailinator.com</t>
+  </si>
+  <si>
+    <t>TC0045_DRACO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UAT_test1 </t>
+  </si>
+  <si>
+    <t>Contact_forUAT</t>
+  </si>
+  <si>
+    <t>uat_test13@mailinator.com</t>
+  </si>
+  <si>
+    <t>TC0046_DRACO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">testiips </t>
+  </si>
+  <si>
+    <t>demo2</t>
+  </si>
+  <si>
+    <t>testdlt1@mail.com</t>
+  </si>
+  <si>
+    <t>TC0047_DRACO</t>
+  </si>
+  <si>
+    <t>testengagement98check98@mailinator.com</t>
+  </si>
+  <si>
+    <t>TC0048_DRACO</t>
+  </si>
+  <si>
+    <t>AutomationMPdraco3</t>
+  </si>
+  <si>
+    <t>Useripa03</t>
+  </si>
+  <si>
+    <t>TC0049_DRACO</t>
+  </si>
+  <si>
+    <t>AutomationMPdraco4</t>
+  </si>
+  <si>
+    <t>TC0050_DRACO</t>
+  </si>
+  <si>
+    <t>AutomationMPdraco5</t>
+  </si>
+  <si>
+    <t>TC0051_DRACO</t>
+  </si>
+  <si>
+    <t>AutomationMPdraco6</t>
+  </si>
+  <si>
+    <t>testqaauto@intel.com.crm.crmqa3</t>
+  </si>
+  <si>
+    <t>Intel*123</t>
   </si>
 </sst>
 </file>
@@ -948,7 +1072,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -1027,6 +1151,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3185,7 +3321,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D3" sqref="D3"/>
+      <selection pane="bottomRight" activeCell="A3" sqref="A3:E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3233,28 +3369,31 @@
         <v>18</v>
       </c>
       <c r="C3" s="28" t="s">
-        <v>220</v>
+        <v>296</v>
       </c>
       <c r="D3" s="29" t="s">
-        <v>221</v>
+        <v>297</v>
       </c>
       <c r="E3" s="1"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:E3" xr:uid="{B30C7179-49C6-4CE4-9EE3-050BEF570246}"/>
   <phoneticPr fontId="3" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="C3" r:id="rId1" xr:uid="{5A420B5D-B2DE-4F29-8D75-44A8298FD4AA}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AE4A502-95AD-4FD1-BDAA-46A877825265}">
-  <dimension ref="A1:P26"/>
+  <dimension ref="A1:R37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D25" sqref="D25"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="L1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="Q1" sqref="Q1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3321,7 +3460,7 @@
         <v>218</v>
       </c>
       <c r="P1" s="34" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.35">
@@ -3335,10 +3474,10 @@
         <v>189</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="E2" s="30" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="F2" s="12" t="str">
         <f>_xlfn.CONCAT(D2,E2,"@mailinator.com")</f>
@@ -3359,13 +3498,13 @@
         <v>189</v>
       </c>
       <c r="D3" s="31" t="s">
+        <v>222</v>
+      </c>
+      <c r="E3" s="31" t="s">
+        <v>223</v>
+      </c>
+      <c r="F3" s="32" t="s">
         <v>224</v>
-      </c>
-      <c r="E3" s="31" t="s">
-        <v>225</v>
-      </c>
-      <c r="F3" s="32" t="s">
-        <v>226</v>
       </c>
       <c r="G3" s="31" t="s">
         <v>195</v>
@@ -3382,10 +3521,10 @@
         <v>189</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="F4" s="12" t="str">
         <f>_xlfn.CONCAT(D4,E4,"@mailinator.com")</f>
@@ -3406,13 +3545,13 @@
         <v>189</v>
       </c>
       <c r="D5" s="31" t="s">
+        <v>225</v>
+      </c>
+      <c r="E5" s="31" t="s">
+        <v>226</v>
+      </c>
+      <c r="F5" s="32" t="s">
         <v>227</v>
-      </c>
-      <c r="E5" s="31" t="s">
-        <v>228</v>
-      </c>
-      <c r="F5" s="32" t="s">
-        <v>229</v>
       </c>
       <c r="G5" s="31" t="s">
         <v>195</v>
@@ -3473,10 +3612,10 @@
         <v>189</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="F10" s="12" t="str">
         <f>_xlfn.CONCAT(D10,E10,"@mailinator.com")</f>
@@ -3486,13 +3625,13 @@
         <v>190</v>
       </c>
       <c r="H10" s="32" t="s">
+        <v>231</v>
+      </c>
+      <c r="I10" s="12" t="s">
+        <v>232</v>
+      </c>
+      <c r="J10" s="12" t="s">
         <v>233</v>
-      </c>
-      <c r="I10" s="12" t="s">
-        <v>234</v>
-      </c>
-      <c r="J10" s="12" t="s">
-        <v>235</v>
       </c>
       <c r="K10" s="12" t="s">
         <v>212</v>
@@ -3509,10 +3648,10 @@
         <v>189</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="F11" s="12" t="str">
         <f>_xlfn.CONCAT(D11,E11,"@mailinator.com")</f>
@@ -3522,7 +3661,7 @@
         <v>190</v>
       </c>
       <c r="H11" s="32" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.35">
@@ -3536,7 +3675,7 @@
         <v>189</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="F12" s="12" t="str">
         <f t="shared" ref="F12:F13" si="0">_xlfn.CONCAT(D12,E12,"@mailinator.com")</f>
@@ -3557,10 +3696,10 @@
         <v>189</v>
       </c>
       <c r="D13" s="12" t="s">
+        <v>237</v>
+      </c>
+      <c r="E13" s="12" t="s">
         <v>239</v>
-      </c>
-      <c r="E13" s="12" t="s">
-        <v>241</v>
       </c>
       <c r="F13" s="12" t="str">
         <f t="shared" si="0"/>
@@ -3570,13 +3709,13 @@
         <v>190</v>
       </c>
       <c r="H13" s="32" t="s">
+        <v>240</v>
+      </c>
+      <c r="I13" s="12" t="s">
+        <v>241</v>
+      </c>
+      <c r="J13" s="12" t="s">
         <v>242</v>
-      </c>
-      <c r="I13" s="12" t="s">
-        <v>243</v>
-      </c>
-      <c r="J13" s="12" t="s">
-        <v>244</v>
       </c>
       <c r="K13" s="12" t="s">
         <v>212</v>
@@ -3621,7 +3760,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A17" s="5" t="s">
         <v>210</v>
       </c>
@@ -3632,7 +3771,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A18" s="5" t="s">
         <v>211</v>
       </c>
@@ -3643,7 +3782,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A19" s="5" t="s">
         <v>213</v>
       </c>
@@ -3654,7 +3793,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A20" s="5" t="s">
         <v>217</v>
       </c>
@@ -3665,7 +3804,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A21" s="5" t="s">
         <v>219</v>
       </c>
@@ -3676,24 +3815,24 @@
         <v>189</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A22" s="33" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A23" s="33" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A24" s="33" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A23" s="33" t="s">
+    <row r="25" spans="1:18" ht="20" x14ac:dyDescent="0.35">
+      <c r="A25" s="33" t="s">
         <v>246</v>
-      </c>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A24" s="33" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="25" spans="1:16" ht="20" x14ac:dyDescent="0.35">
-      <c r="A25" s="33" t="s">
-        <v>248</v>
       </c>
       <c r="B25" s="12" t="s">
         <v>184</v>
@@ -3702,25 +3841,25 @@
         <v>189</v>
       </c>
       <c r="D25" s="12" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="E25" s="30" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="F25" s="12" t="str">
         <f>_xlfn.CONCAT(D25,E25,"@mailinator.com")</f>
         <v>AutomationMPdraco2Useripa02@mailinator.com</v>
       </c>
       <c r="G25" s="30" t="s">
+        <v>250</v>
+      </c>
+      <c r="P25" s="35" t="s">
         <v>252</v>
       </c>
-      <c r="P25" s="35" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="26" spans="1:16" ht="30" x14ac:dyDescent="0.35">
+    </row>
+    <row r="26" spans="1:18" ht="20" x14ac:dyDescent="0.35">
       <c r="A26" s="33" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="B26" s="12" t="s">
         <v>184</v>
@@ -3729,20 +3868,484 @@
         <v>189</v>
       </c>
       <c r="D26" s="12" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="E26" s="30" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="F26" s="12" t="str">
         <f>_xlfn.CONCAT(D26,E26,"@mailinator.com")</f>
         <v>AutomationMPdracoUseripa01@mailinator.com</v>
       </c>
       <c r="G26" s="30" t="s">
+        <v>250</v>
+      </c>
+      <c r="P26" s="35" t="s">
         <v>252</v>
       </c>
-      <c r="P26" s="35" t="s">
+    </row>
+    <row r="27" spans="1:18" ht="29" x14ac:dyDescent="0.35">
+      <c r="A27" s="5" t="s">
+        <v>255</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="F27" s="36" t="s">
+        <v>258</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="H27" s="2"/>
+      <c r="I27" s="2"/>
+      <c r="J27" s="2"/>
+      <c r="K27" s="2"/>
+      <c r="L27" s="2"/>
+      <c r="M27" s="2"/>
+      <c r="N27" s="2"/>
+      <c r="O27" s="2"/>
+      <c r="P27" s="37" t="s">
+        <v>252</v>
+      </c>
+      <c r="Q27" s="3" t="s">
+        <v>260</v>
+      </c>
+      <c r="R27" s="2" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" ht="29" x14ac:dyDescent="0.35">
+      <c r="A28" s="5" t="s">
+        <v>262</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="F28" s="38" t="s">
+        <v>265</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="H28" s="2"/>
+      <c r="I28" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="J28" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="K28" s="2"/>
+      <c r="L28" s="2"/>
+      <c r="M28" s="2"/>
+      <c r="N28" s="2"/>
+      <c r="O28" s="2"/>
+      <c r="P28" s="39" t="s">
+        <v>252</v>
+      </c>
+      <c r="Q28" s="3" t="s">
+        <v>268</v>
+      </c>
+      <c r="R28" s="2" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" ht="20" x14ac:dyDescent="0.35">
+      <c r="A29" s="5" t="s">
+        <v>269</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="F29" s="38" t="s">
+        <v>265</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="H29" s="2"/>
+      <c r="I29" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="J29" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="K29" s="2"/>
+      <c r="L29" s="2"/>
+      <c r="M29" s="2"/>
+      <c r="N29" s="2"/>
+      <c r="O29" s="2"/>
+      <c r="P29" s="37" t="s">
+        <v>252</v>
+      </c>
+      <c r="Q29" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="R29" s="2" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" ht="20" x14ac:dyDescent="0.35">
+      <c r="A30" s="5" t="s">
+        <v>273</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="F30" s="38" t="s">
+        <v>265</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="H30" s="2"/>
+      <c r="I30" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="J30" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="K30" s="2"/>
+      <c r="L30" s="2"/>
+      <c r="M30" s="2"/>
+      <c r="N30" s="2"/>
+      <c r="O30" s="2"/>
+      <c r="P30" s="37" t="s">
+        <v>252</v>
+      </c>
+      <c r="Q30" s="3" t="s">
+        <v>276</v>
+      </c>
+      <c r="R30" s="2" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" ht="20" x14ac:dyDescent="0.35">
+      <c r="A31" s="5" t="s">
+        <v>277</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="F31" s="38" t="s">
+        <v>265</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="H31" s="2"/>
+      <c r="I31" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="J31" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="K31" s="2"/>
+      <c r="L31" s="2"/>
+      <c r="M31" s="2"/>
+      <c r="N31" s="2"/>
+      <c r="O31" s="2"/>
+      <c r="P31" s="37" t="s">
+        <v>252</v>
+      </c>
+      <c r="Q31" s="3" t="s">
+        <v>280</v>
+      </c>
+      <c r="R31" s="2" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" ht="20" x14ac:dyDescent="0.35">
+      <c r="A32" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="F32" s="38" t="s">
+        <v>265</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="H32" s="2"/>
+      <c r="I32" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="J32" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="K32" s="2"/>
+      <c r="L32" s="2"/>
+      <c r="M32" s="2"/>
+      <c r="N32" s="2"/>
+      <c r="O32" s="2"/>
+      <c r="P32" s="37" t="s">
+        <v>252</v>
+      </c>
+      <c r="Q32" s="3" t="s">
+        <v>284</v>
+      </c>
+      <c r="R32" s="2" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="33" spans="1:18" ht="20" x14ac:dyDescent="0.35">
+      <c r="A33" s="5" t="s">
+        <v>285</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="F33" s="38" t="s">
+        <v>265</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="H33" s="2"/>
+      <c r="I33" s="2"/>
+      <c r="J33" s="2"/>
+      <c r="K33" s="2"/>
+      <c r="L33" s="2"/>
+      <c r="M33" s="2"/>
+      <c r="N33" s="2"/>
+      <c r="O33" s="2"/>
+      <c r="P33" s="37" t="s">
+        <v>252</v>
+      </c>
+      <c r="Q33" s="32" t="s">
+        <v>286</v>
+      </c>
+      <c r="R33" s="2" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="34" spans="1:18" ht="20" x14ac:dyDescent="0.35">
+      <c r="A34" s="5" t="s">
+        <v>287</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="F34" s="2" t="str">
+        <f>_xlfn.CONCAT(D34,E34,"@mailinator.com")</f>
+        <v>AutomationMPdraco3Useripa03@mailinator.com</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="H34" s="2"/>
+      <c r="I34" s="2"/>
+      <c r="J34" s="2"/>
+      <c r="K34" s="2"/>
+      <c r="L34" s="2"/>
+      <c r="M34" s="2"/>
+      <c r="N34" s="2"/>
+      <c r="O34" s="2"/>
+      <c r="P34" s="37" t="s">
+        <v>252</v>
+      </c>
+      <c r="Q34" s="32" t="s">
+        <v>286</v>
+      </c>
+      <c r="R34" s="2" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="35" spans="1:18" ht="20" x14ac:dyDescent="0.35">
+      <c r="A35" s="5" t="s">
+        <v>290</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="F35" s="2" t="str">
+        <f>_xlfn.CONCAT(D35,E35,"@mailinator.com")</f>
+        <v>AutomationMPdraco4Useripa03@mailinator.com</v>
+      </c>
+      <c r="G35" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="H35" s="2"/>
+      <c r="I35" s="2"/>
+      <c r="J35" s="2"/>
+      <c r="K35" s="2"/>
+      <c r="L35" s="2"/>
+      <c r="M35" s="2"/>
+      <c r="N35" s="2"/>
+      <c r="O35" s="2"/>
+      <c r="P35" s="37" t="s">
+        <v>252</v>
+      </c>
+      <c r="Q35" s="32" t="s">
+        <v>286</v>
+      </c>
+      <c r="R35" s="2" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="36" spans="1:18" ht="20" x14ac:dyDescent="0.35">
+      <c r="A36" s="5" t="s">
+        <v>292</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="E36" s="2" t="s">
         <v>254</v>
+      </c>
+      <c r="F36" s="2" t="str">
+        <f>_xlfn.CONCAT(D36,E36,"@mailinator.com")</f>
+        <v>AutomationMPdraco5Useripa02@mailinator.com</v>
+      </c>
+      <c r="G36" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="H36" s="2"/>
+      <c r="I36" s="2"/>
+      <c r="J36" s="2"/>
+      <c r="K36" s="2"/>
+      <c r="L36" s="2"/>
+      <c r="M36" s="2"/>
+      <c r="N36" s="2"/>
+      <c r="O36" s="2"/>
+      <c r="P36" s="37" t="s">
+        <v>252</v>
+      </c>
+      <c r="Q36" s="32" t="s">
+        <v>286</v>
+      </c>
+      <c r="R36" s="2" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="37" spans="1:18" ht="20" x14ac:dyDescent="0.35">
+      <c r="A37" s="5" t="s">
+        <v>294</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="F37" s="2" t="str">
+        <f>_xlfn.CONCAT(D37,E37,"@mailinator.com")</f>
+        <v>AutomationMPdraco6Useripa02@mailinator.com</v>
+      </c>
+      <c r="G37" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="H37" s="2"/>
+      <c r="I37" s="2"/>
+      <c r="J37" s="2"/>
+      <c r="K37" s="2"/>
+      <c r="L37" s="2"/>
+      <c r="M37" s="2"/>
+      <c r="N37" s="2"/>
+      <c r="O37" s="2"/>
+      <c r="P37" s="37" t="s">
+        <v>252</v>
+      </c>
+      <c r="Q37" s="32" t="s">
+        <v>286</v>
+      </c>
+      <c r="R37" s="2" t="s">
+        <v>261</v>
       </c>
     </row>
   </sheetData>
@@ -3753,8 +4356,26 @@
     <hyperlink ref="H10" r:id="rId3" xr:uid="{DD0408AB-2BA5-4990-B211-0DF01180EEC9}"/>
     <hyperlink ref="H11" r:id="rId4" display="mailto:test_qa0922@mailinator.com" xr:uid="{F8176DC2-7FD5-4C57-A0BD-03F4F7642923}"/>
     <hyperlink ref="H13" r:id="rId5" xr:uid="{47E4F6EA-292A-4519-B99F-6843185CD22E}"/>
+    <hyperlink ref="Q27" r:id="rId6" xr:uid="{8AC9AF0A-2A47-46DA-8FCB-77580023A2D8}"/>
+    <hyperlink ref="Q28" r:id="rId7" xr:uid="{A8D313D5-882C-4B6A-AAC9-0DB7DA60759D}"/>
+    <hyperlink ref="Q30" r:id="rId8" xr:uid="{A1D308F4-98D3-4F7D-80BC-4FF8D0F1590A}"/>
+    <hyperlink ref="Q31" r:id="rId9" xr:uid="{893F6EE2-D894-4B19-8B0F-2E12288175B7}"/>
+    <hyperlink ref="Q32" r:id="rId10" xr:uid="{7F400370-81C9-452A-865D-37373A7C04D0}"/>
+    <hyperlink ref="Q29" r:id="rId11" xr:uid="{9BBB1257-7F9E-4CA8-90E5-2C7B989B8257}"/>
+    <hyperlink ref="F28" r:id="rId12" xr:uid="{650E7A69-1E7E-4F5C-8679-C8470315F881}"/>
+    <hyperlink ref="P28" r:id="rId13" xr:uid="{E2E6EA6E-5BE3-48F5-9F6A-1A8B70A07695}"/>
+    <hyperlink ref="F29" r:id="rId14" xr:uid="{EFE4F115-3128-437A-A59A-FE02B81BC722}"/>
+    <hyperlink ref="F30" r:id="rId15" xr:uid="{F7CB1880-1F97-475D-A862-B556B6DFAA6A}"/>
+    <hyperlink ref="F31" r:id="rId16" xr:uid="{DB82769F-5CE2-4B86-B435-A9E4417614D4}"/>
+    <hyperlink ref="F32" r:id="rId17" xr:uid="{37D84B70-DD44-478B-BB84-5F478EA90D3C}"/>
+    <hyperlink ref="Q33" r:id="rId18" xr:uid="{486BF87D-4AFC-4AB9-8D54-F7F293061449}"/>
+    <hyperlink ref="F33" r:id="rId19" xr:uid="{9DFDA37D-2143-4805-BDC2-BACD2CC22842}"/>
+    <hyperlink ref="Q34" r:id="rId20" xr:uid="{23C11847-CFF5-4E21-8AC2-4C009B12F4E3}"/>
+    <hyperlink ref="Q36" r:id="rId21" xr:uid="{796AA88E-2164-453F-9E2D-480755763345}"/>
+    <hyperlink ref="Q37" r:id="rId22" xr:uid="{72BCEEA9-1C08-487D-ADAA-9167BF9D1D1A}"/>
+    <hyperlink ref="Q35" r:id="rId23" xr:uid="{E16CE575-3E79-4A4F-9830-310D8C16A1BE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId6"/>
+  <pageSetup orientation="portrait" r:id="rId24"/>
 </worksheet>
 </file>
</xml_diff>